<commit_message>
LC Tracking - 4/4/24
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EB5425-B24A-314D-BDF7-42AABF1F2F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAA7207-E862-0D44-975F-86B604F0D946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="331">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1004,13 +1004,31 @@
     <t>Maximum Nesting Depth of the Parentheses</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/maximum-nesting-depth-of-the-parentheses/</t>
-  </si>
-  <si>
     <t>Stack</t>
   </si>
   <si>
     <t>Keep stack of open parens and store max when match happens, if no parens return 0 otherwise return max</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-nesting-depth-of-the-parentheses/submissions/1222840733/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of Matches in Tournament </t>
+  </si>
+  <si>
+    <t>Just follow formulas in description, keep cutting players in half and summing matches</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-of-matches-in-tournament/submissions/1222847215/</t>
+  </si>
+  <si>
+    <t>Minimum Number of Swaps to Make The Binary String Alternating</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-number-of-swaps-to-make-the-binary-string-alternating/submissions/1223657856/</t>
+  </si>
+  <si>
+    <t>Break into cases, either starts w 0 or 1, count number of pairs of incorrect placings based on string</t>
   </si>
 </sst>
 </file>
@@ -1437,15 +1455,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.5" customWidth="1"/>
+    <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
@@ -3003,6 +3021,9 @@
       <c r="F67" s="3" t="s">
         <v>105</v>
       </c>
+      <c r="G67" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
@@ -3017,6 +3038,9 @@
       <c r="F68" s="3" t="s">
         <v>105</v>
       </c>
+      <c r="G68" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -3756,19 +3780,65 @@
         <v>96</v>
       </c>
       <c r="C101" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D101" t="s">
+        <v>323</v>
+      </c>
+      <c r="E101" s="3">
+        <v>1</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G101" t="s">
         <v>322</v>
       </c>
-      <c r="D101" t="s">
-        <v>324</v>
-      </c>
-      <c r="E101" s="3">
-        <v>1</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G101" t="s">
-        <v>323</v>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>325</v>
+      </c>
+      <c r="B102" t="s">
+        <v>96</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D102" t="s">
+        <v>326</v>
+      </c>
+      <c r="E102" s="3">
+        <v>1</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G102" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>328</v>
+      </c>
+      <c r="B103" t="s">
+        <v>94</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D103" t="s">
+        <v>330</v>
+      </c>
+      <c r="E103" s="3">
+        <v>1</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G103" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3792,6 +3862,8 @@
     <hyperlink ref="C54" r:id="rId6" xr:uid="{56C2A67E-F040-E441-9AAD-EDDB6B56167F}"/>
     <hyperlink ref="C100" r:id="rId7" xr:uid="{2E00D544-656B-474A-88A0-060265C5B930}"/>
     <hyperlink ref="C101" r:id="rId8" xr:uid="{EB62723E-BA7C-BC44-9ACD-730F166AC739}"/>
+    <hyperlink ref="C102" r:id="rId9" xr:uid="{1D3CE224-10BD-054D-989C-6C5AE62BD32C}"/>
+    <hyperlink ref="C103" r:id="rId10" xr:uid="{70A93119-9023-B243-9119-FC3BE9D5AA95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 4/7/24
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAA7207-E862-0D44-975F-86B604F0D946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A24E242-955A-2B41-A71C-683FE156850D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="337">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1029,6 +1029,24 @@
   </si>
   <si>
     <t>Break into cases, either starts w 0 or 1, count number of pairs of incorrect placings based on string</t>
+  </si>
+  <si>
+    <t>Make the String Great</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/make-the-string-great/submissions/1223730717/</t>
+  </si>
+  <si>
+    <t>Use stack to keep track of matching letters, return string that is reverse of stack at end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum Remove to Make Valid Parentheses </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-remove-to-make-valid-parentheses/submissions/1225488024/</t>
+  </si>
+  <si>
+    <t>Use stack to push only open parens, if empty stack and closing invalid index, opens at end also invalid</t>
   </si>
 </sst>
 </file>
@@ -1455,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A78" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3839,6 +3857,52 @@
       </c>
       <c r="G103" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>331</v>
+      </c>
+      <c r="B104" t="s">
+        <v>96</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D104" t="s">
+        <v>333</v>
+      </c>
+      <c r="E104" s="3">
+        <v>1</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G104" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>334</v>
+      </c>
+      <c r="B105" t="s">
+        <v>94</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D105" t="s">
+        <v>336</v>
+      </c>
+      <c r="E105" s="3">
+        <v>1</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G105" t="s">
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -3864,6 +3928,8 @@
     <hyperlink ref="C101" r:id="rId8" xr:uid="{EB62723E-BA7C-BC44-9ACD-730F166AC739}"/>
     <hyperlink ref="C102" r:id="rId9" xr:uid="{1D3CE224-10BD-054D-989C-6C5AE62BD32C}"/>
     <hyperlink ref="C103" r:id="rId10" xr:uid="{70A93119-9023-B243-9119-FC3BE9D5AA95}"/>
+    <hyperlink ref="C104" r:id="rId11" xr:uid="{AE38C7E2-00A6-8646-A12D-AFF181BCF262}"/>
+    <hyperlink ref="C105" r:id="rId12" xr:uid="{D55FC07F-524D-B941-8C22-52898EB4771E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 4/18
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A24E242-955A-2B41-A71C-683FE156850D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C355459-EAE9-AC46-8C71-35DF78909C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="346">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1004,9 +1004,6 @@
     <t>Maximum Nesting Depth of the Parentheses</t>
   </si>
   <si>
-    <t>Stack</t>
-  </si>
-  <si>
     <t>Keep stack of open parens and store max when match happens, if no parens return 0 otherwise return max</t>
   </si>
   <si>
@@ -1047,6 +1044,36 @@
   </si>
   <si>
     <t>Use stack to push only open parens, if empty stack and closing invalid index, opens at end also invalid</t>
+  </si>
+  <si>
+    <t>Valid Parenthesis String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-parenthesis-string/submissions/1226316842/</t>
+  </si>
+  <si>
+    <t>Keep two index stacks for * and (, pop when you see ), go through stacks and if ( index ever more than * index, return false</t>
+  </si>
+  <si>
+    <t>Time Needed to Buy Tickets</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/time-needed-to-buy-tickets/submissions/1227961938/</t>
+  </si>
+  <si>
+    <t>Use a deque to simulate problem, store both tickets left and index</t>
+  </si>
+  <si>
+    <t>Stack or Queue</t>
+  </si>
+  <si>
+    <t>Island Perimeter</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/island-perimeter/submissions/1235470710/</t>
+  </si>
+  <si>
+    <t>Increment by perimeter by 4 always, detract 1 for each neighboring island chunk</t>
   </si>
 </sst>
 </file>
@@ -1473,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3798,10 +3825,10 @@
         <v>96</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D101" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E101" s="3">
         <v>1</v>
@@ -3810,21 +3837,21 @@
         <v>7</v>
       </c>
       <c r="G101" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B102" t="s">
         <v>96</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D102" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E102" s="3">
         <v>1</v>
@@ -3838,16 +3865,16 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>327</v>
+      </c>
+      <c r="B103" t="s">
+        <v>94</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B103" t="s">
-        <v>94</v>
-      </c>
-      <c r="C103" s="2" t="s">
+      <c r="D103" t="s">
         <v>329</v>
-      </c>
-      <c r="D103" t="s">
-        <v>330</v>
       </c>
       <c r="E103" s="3">
         <v>1</v>
@@ -3861,17 +3888,17 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B104" t="s">
         <v>96</v>
       </c>
       <c r="C104" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D104" t="s">
         <v>332</v>
       </c>
-      <c r="D104" t="s">
-        <v>333</v>
-      </c>
       <c r="E104" s="3">
         <v>1</v>
       </c>
@@ -3879,30 +3906,99 @@
         <v>7</v>
       </c>
       <c r="G104" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>333</v>
+      </c>
+      <c r="B105" t="s">
+        <v>94</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B105" t="s">
-        <v>94</v>
-      </c>
-      <c r="C105" s="2" t="s">
+      <c r="D105" t="s">
         <v>335</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" s="3">
+        <v>1</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G105" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>336</v>
       </c>
-      <c r="E105" s="3">
-        <v>1</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G105" t="s">
-        <v>322</v>
+      <c r="B106" t="s">
+        <v>94</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D106" t="s">
+        <v>338</v>
+      </c>
+      <c r="E106" s="3">
+        <v>1</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G106" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>339</v>
+      </c>
+      <c r="B107" t="s">
+        <v>96</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D107" t="s">
+        <v>341</v>
+      </c>
+      <c r="E107" s="3">
+        <v>1</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G107" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>343</v>
+      </c>
+      <c r="B108" t="s">
+        <v>96</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D108" t="s">
+        <v>345</v>
+      </c>
+      <c r="E108" s="3">
+        <v>1</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G108" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3930,6 +4026,9 @@
     <hyperlink ref="C103" r:id="rId10" xr:uid="{70A93119-9023-B243-9119-FC3BE9D5AA95}"/>
     <hyperlink ref="C104" r:id="rId11" xr:uid="{AE38C7E2-00A6-8646-A12D-AFF181BCF262}"/>
     <hyperlink ref="C105" r:id="rId12" xr:uid="{D55FC07F-524D-B941-8C22-52898EB4771E}"/>
+    <hyperlink ref="C106" r:id="rId13" xr:uid="{ACB585E1-7727-F247-AE00-6D19E577064C}"/>
+    <hyperlink ref="C107" r:id="rId14" xr:uid="{43B1F1E3-061F-6F4F-9330-8E8D5B03E3E9}"/>
+    <hyperlink ref="C108" r:id="rId15" xr:uid="{45971529-0C3A-314D-BB31-CCCDE4921AB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 4/19
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C355459-EAE9-AC46-8C71-35DF78909C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D12C7E-8D21-AE45-BF0C-BC6B9C0C1F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="349">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1074,6 +1074,15 @@
   </si>
   <si>
     <t>Increment by perimeter by 4 always, detract 1 for each neighboring island chunk</t>
+  </si>
+  <si>
+    <t>Number of Islands</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-islands/submissions/1236373928/</t>
+  </si>
+  <si>
+    <t>Do DFS on '1', set cell to visited and do DFS on adjacent cell, increment for each call</t>
   </si>
 </sst>
 </file>
@@ -1500,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:J108"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3999,6 +4008,29 @@
       </c>
       <c r="G108" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>346</v>
+      </c>
+      <c r="B109" t="s">
+        <v>94</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D109" t="s">
+        <v>348</v>
+      </c>
+      <c r="E109" s="3">
+        <v>1</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G109" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -4029,6 +4061,7 @@
     <hyperlink ref="C106" r:id="rId13" xr:uid="{ACB585E1-7727-F247-AE00-6D19E577064C}"/>
     <hyperlink ref="C107" r:id="rId14" xr:uid="{43B1F1E3-061F-6F4F-9330-8E8D5B03E3E9}"/>
     <hyperlink ref="C108" r:id="rId15" xr:uid="{45971529-0C3A-314D-BB31-CCCDE4921AB5}"/>
+    <hyperlink ref="C109" r:id="rId16" xr:uid="{C3A446B8-F146-1D4D-8A9F-EF8B8ACAB0AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 4/25
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D12C7E-8D21-AE45-BF0C-BC6B9C0C1F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B4AFBC-AF50-E642-92D2-27F689FB07F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="364">
   <si>
     <t>Problem Name</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Store cumulative 1 counts vertically, find largest submatrix going row by row in new matrix</t>
   </si>
   <si>
-    <t>Use bottom up DP, store previous and current state for each position, have map of neighbors</t>
-  </si>
-  <si>
     <t>Transpose Matrix</t>
   </si>
   <si>
@@ -773,9 +770,6 @@
     <t>https://leetcode.com/problems/largest-submatrix-with-rearrangements/submissions/1106965425/</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/knight-dialer/submissions/1107585991/</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/transpose-matrix/submissions/1116795685/</t>
   </si>
   <si>
@@ -1083,6 +1077,57 @@
   </si>
   <si>
     <t>Do DFS on '1', set cell to visited and do DFS on adjacent cell, increment for each call</t>
+  </si>
+  <si>
+    <t>Consecutive Numbers Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/consecutive-numbers-sum/submissions/1236422244/</t>
+  </si>
+  <si>
+    <t>Loop from 2 … sqrt(2n), check if n - (natural number sum up to i) divisible by i</t>
+  </si>
+  <si>
+    <t>Longest String Chain</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-string-chain/submissions/1238833054/</t>
+  </si>
+  <si>
+    <t>Sort words by size, keep dp arr and do n^2 loop to check character pairs that are 1 apart to see if valid, keep track of longest chain</t>
+  </si>
+  <si>
+    <t>Different Ways to Add Parentheses</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/different-ways-to-add-parentheses/submissions/1239358596/</t>
+  </si>
+  <si>
+    <t>Recursive l,r tree splitting string at each index, compute expression and push back to result every step</t>
+  </si>
+  <si>
+    <t>Palindromic Substrings</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindromic-substrings/submissions/1239369036/</t>
+  </si>
+  <si>
+    <t>Expand from middle, check both odd and even and just increment count while chars are equal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-valid-parentheses/submissions/1240498853/</t>
+  </si>
+  <si>
+    <t>Longest Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Store array, whenever you encounter valid paren pairs, convert corr. Index in arr to same symbol, find longest contiguous occurrences of symbol</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/knight-dialer/submissions/1241442723/</t>
+  </si>
+  <si>
+    <t>Top down DP, keep dp[10][n+1], just go through each neighbor for each index till n one, store and update result</t>
   </si>
 </sst>
 </file>
@@ -1509,10 +1554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1532,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1551,10 +1596,10 @@
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1562,10 +1607,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -1583,7 +1628,7 @@
         <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1591,10 +1636,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1612,7 +1657,7 @@
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1620,13 +1665,13 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1635,13 +1680,13 @@
         <v>6</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1649,10 +1694,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -1672,10 +1717,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -1695,10 +1740,10 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -1718,10 +1763,10 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -1741,10 +1786,10 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
@@ -1764,10 +1809,10 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -1787,10 +1832,10 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
@@ -1802,7 +1847,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1810,10 +1855,10 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D12" t="s">
         <v>31</v>
@@ -1833,10 +1878,10 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
@@ -1846,7 +1891,7 @@
         <v>6</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1854,10 +1899,10 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D14" t="s">
         <v>36</v>
@@ -1877,10 +1922,10 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D15" t="s">
         <v>38</v>
@@ -1900,10 +1945,10 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D16" t="s">
         <v>40</v>
@@ -1923,10 +1968,10 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D17" t="s">
         <v>42</v>
@@ -1946,10 +1991,10 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D18" t="s">
         <v>44</v>
@@ -1969,10 +2014,10 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D19" t="s">
         <v>46</v>
@@ -1992,10 +2037,10 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D20" t="s">
         <v>48</v>
@@ -2012,13 +2057,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D21" t="s">
         <v>50</v>
@@ -2038,10 +2083,10 @@
         <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D22" t="s">
         <v>52</v>
@@ -2061,10 +2106,10 @@
         <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D23" t="s">
         <v>55</v>
@@ -2084,36 +2129,36 @@
         <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>245</v>
+        <v>362</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>363</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D25" t="s">
         <v>57</v>
-      </c>
-      <c r="B25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D25" t="s">
-        <v>58</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2127,16 +2172,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D26" t="s">
         <v>59</v>
-      </c>
-      <c r="B26" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D26" t="s">
-        <v>60</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -2150,16 +2195,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D27" t="s">
         <v>61</v>
-      </c>
-      <c r="B27" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="D27" t="s">
-        <v>62</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -2173,16 +2218,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -2196,16 +2241,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D29" t="s">
         <v>65</v>
-      </c>
-      <c r="B29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D29" t="s">
-        <v>66</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -2214,22 +2259,22 @@
         <v>6</v>
       </c>
       <c r="G29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D30" t="s">
         <v>68</v>
       </c>
-      <c r="B30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D30" t="s">
-        <v>69</v>
-      </c>
       <c r="E30">
         <v>1</v>
       </c>
@@ -2237,21 +2282,21 @@
         <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D31" t="s">
         <v>70</v>
-      </c>
-      <c r="B31" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D31" t="s">
-        <v>71</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -2265,16 +2310,16 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D32" t="s">
         <v>72</v>
-      </c>
-      <c r="B32" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D32" t="s">
-        <v>73</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -2288,16 +2333,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D33" t="s">
         <v>74</v>
-      </c>
-      <c r="B33" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D33" t="s">
-        <v>75</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -2311,16 +2356,16 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D34" t="s">
         <v>76</v>
-      </c>
-      <c r="B34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D34" t="s">
-        <v>77</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -2334,17 +2379,17 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" t="s">
         <v>78</v>
       </c>
-      <c r="B35" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="D35" t="s">
-        <v>79</v>
-      </c>
       <c r="E35">
         <v>1</v>
       </c>
@@ -2352,21 +2397,21 @@
         <v>7</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D36" t="s">
         <v>80</v>
-      </c>
-      <c r="B36" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D36" t="s">
-        <v>81</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -2380,16 +2425,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D37" t="s">
         <v>82</v>
-      </c>
-      <c r="B37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" t="s">
-        <v>83</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -2403,16 +2448,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D38" t="s">
         <v>84</v>
-      </c>
-      <c r="B38" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="D38" t="s">
-        <v>85</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -2426,17 +2471,17 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" t="s">
         <v>87</v>
       </c>
-      <c r="B39" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="D39" t="s">
-        <v>88</v>
-      </c>
       <c r="E39">
         <v>1</v>
       </c>
@@ -2444,21 +2489,21 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D40" t="s">
         <v>89</v>
-      </c>
-      <c r="B40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="D40" t="s">
-        <v>90</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -2472,16 +2517,16 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D41" t="s">
         <v>91</v>
-      </c>
-      <c r="B41" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="D41" t="s">
-        <v>92</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -2495,16 +2540,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E42" s="3">
         <v>1</v>
@@ -2518,16 +2563,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E43" s="3">
         <v>1</v>
@@ -2536,21 +2581,21 @@
         <v>7</v>
       </c>
       <c r="G43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D44" t="s">
         <v>102</v>
-      </c>
-      <c r="B44" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="D44" t="s">
-        <v>103</v>
       </c>
       <c r="E44" s="3">
         <v>1</v>
@@ -2564,16 +2609,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E45" s="3">
         <v>1</v>
@@ -2587,16 +2632,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E46" s="3">
         <v>1</v>
@@ -2605,21 +2650,21 @@
         <v>6</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D47" t="s">
         <v>109</v>
-      </c>
-      <c r="B47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="D47" t="s">
-        <v>110</v>
       </c>
       <c r="E47" s="3">
         <v>2</v>
@@ -2628,21 +2673,21 @@
         <v>7</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E48" s="3">
         <v>3</v>
@@ -2651,22 +2696,22 @@
         <v>7</v>
       </c>
       <c r="G48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D49" t="s">
         <v>114</v>
       </c>
-      <c r="B49" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D49" t="s">
-        <v>115</v>
-      </c>
       <c r="E49" s="3">
         <v>1</v>
       </c>
@@ -2674,21 +2719,21 @@
         <v>7</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D50" t="s">
         <v>116</v>
-      </c>
-      <c r="B50" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D50" t="s">
-        <v>117</v>
       </c>
       <c r="E50" s="3">
         <v>1</v>
@@ -2702,59 +2747,59 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D51" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" t="s">
         <v>120</v>
-      </c>
-      <c r="B51" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D51" t="s">
-        <v>122</v>
-      </c>
-      <c r="E51" s="3">
-        <v>1</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E52" s="3">
         <v>1</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E53" s="3">
         <v>1</v>
@@ -2763,41 +2808,41 @@
         <v>6</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B54" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="E54" s="3">
         <v>1</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E55" s="3">
         <v>1</v>
@@ -2806,21 +2851,21 @@
         <v>7</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D56" t="s">
         <v>128</v>
-      </c>
-      <c r="B56" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D56" t="s">
-        <v>129</v>
       </c>
       <c r="E56" s="3">
         <v>1</v>
@@ -2834,16 +2879,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E57" s="3">
         <v>1</v>
@@ -2857,16 +2902,16 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D58" t="s">
         <v>133</v>
-      </c>
-      <c r="B58" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D58" t="s">
-        <v>134</v>
       </c>
       <c r="E58" s="3">
         <v>1</v>
@@ -2880,16 +2925,16 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D59" t="s">
         <v>135</v>
-      </c>
-      <c r="B59" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D59" t="s">
-        <v>136</v>
       </c>
       <c r="E59" s="3">
         <v>1</v>
@@ -2898,22 +2943,22 @@
         <v>6</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D60" t="s">
         <v>138</v>
       </c>
-      <c r="B60" t="s">
-        <v>96</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="D60" t="s">
-        <v>139</v>
-      </c>
       <c r="E60" s="3">
         <v>1</v>
       </c>
@@ -2921,21 +2966,21 @@
         <v>7</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D61" t="s">
         <v>140</v>
-      </c>
-      <c r="B61" t="s">
-        <v>94</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D61" t="s">
-        <v>141</v>
       </c>
       <c r="E61" s="3">
         <v>1</v>
@@ -2949,17 +2994,17 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D62" t="s">
         <v>142</v>
       </c>
-      <c r="B62" t="s">
-        <v>96</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D62" t="s">
-        <v>143</v>
-      </c>
       <c r="E62" s="3">
         <v>1</v>
       </c>
@@ -2967,22 +3012,22 @@
         <v>7</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D63" t="s">
         <v>144</v>
       </c>
-      <c r="B63" t="s">
-        <v>96</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D63" t="s">
-        <v>145</v>
-      </c>
       <c r="E63" s="3">
         <v>1</v>
       </c>
@@ -2990,22 +3035,22 @@
         <v>7</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>145</v>
+      </c>
+      <c r="B64" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D64" t="s">
         <v>146</v>
       </c>
-      <c r="B64" t="s">
-        <v>96</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D64" t="s">
-        <v>147</v>
-      </c>
       <c r="E64" s="3">
         <v>1</v>
       </c>
@@ -3013,21 +3058,21 @@
         <v>7</v>
       </c>
       <c r="G64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" t="s">
+        <v>93</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D65" t="s">
         <v>148</v>
-      </c>
-      <c r="B65" t="s">
-        <v>94</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D65" t="s">
-        <v>149</v>
       </c>
       <c r="E65" s="3">
         <v>1</v>
@@ -3036,21 +3081,21 @@
         <v>6</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>149</v>
+      </c>
+      <c r="B66" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D66" t="s">
         <v>150</v>
-      </c>
-      <c r="B66" t="s">
-        <v>94</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D66" t="s">
-        <v>151</v>
       </c>
       <c r="E66" s="3">
         <v>1</v>
@@ -3064,16 +3109,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" t="s">
+        <v>93</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B67" t="s">
-        <v>94</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="F67" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G67" t="s">
         <v>49</v>
@@ -3081,16 +3126,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G68" t="s">
         <v>49</v>
@@ -3098,16 +3143,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D69" t="s">
         <v>156</v>
-      </c>
-      <c r="B69" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="D69" t="s">
-        <v>157</v>
       </c>
       <c r="E69" s="3">
         <v>1</v>
@@ -3116,21 +3161,21 @@
         <v>6</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>157</v>
+      </c>
+      <c r="B70" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D70" t="s">
         <v>158</v>
-      </c>
-      <c r="B70" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="D70" t="s">
-        <v>159</v>
       </c>
       <c r="E70" s="3">
         <v>1</v>
@@ -3139,45 +3184,45 @@
         <v>6</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>159</v>
+      </c>
+      <c r="B71" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D71" t="s">
         <v>160</v>
       </c>
-      <c r="B71" t="s">
-        <v>96</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" s="3">
+        <v>1</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" t="s">
         <v>161</v>
-      </c>
-      <c r="E71" s="3">
-        <v>1</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G71" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>162</v>
+      </c>
+      <c r="B72" t="s">
+        <v>95</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D72" t="s">
         <v>163</v>
       </c>
-      <c r="B72" t="s">
-        <v>96</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D72" t="s">
-        <v>164</v>
-      </c>
       <c r="E72" s="3">
         <v>1</v>
       </c>
@@ -3185,22 +3230,22 @@
         <v>7</v>
       </c>
       <c r="G72" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>164</v>
+      </c>
+      <c r="B73" t="s">
+        <v>93</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D73" t="s">
         <v>165</v>
       </c>
-      <c r="B73" t="s">
-        <v>94</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="D73" t="s">
-        <v>166</v>
-      </c>
       <c r="E73" s="3">
         <v>1</v>
       </c>
@@ -3208,21 +3253,21 @@
         <v>7</v>
       </c>
       <c r="G73" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>166</v>
+      </c>
+      <c r="B74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D74" t="s">
         <v>167</v>
-      </c>
-      <c r="B74" t="s">
-        <v>94</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="D74" t="s">
-        <v>168</v>
       </c>
       <c r="E74" s="3">
         <v>1</v>
@@ -3231,21 +3276,21 @@
         <v>6</v>
       </c>
       <c r="G74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D75" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E75" s="3">
         <v>1</v>
@@ -3254,21 +3299,21 @@
         <v>7</v>
       </c>
       <c r="G75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D76" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E76" s="3">
         <v>1</v>
@@ -3277,22 +3322,22 @@
         <v>7</v>
       </c>
       <c r="G76" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" t="s">
+        <v>93</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D77" t="s">
         <v>173</v>
       </c>
-      <c r="B77" t="s">
-        <v>94</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D77" t="s">
-        <v>174</v>
-      </c>
       <c r="E77" s="3">
         <v>1</v>
       </c>
@@ -3300,21 +3345,21 @@
         <v>7</v>
       </c>
       <c r="G77" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" t="s">
+        <v>93</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D78" t="s">
         <v>175</v>
-      </c>
-      <c r="B78" t="s">
-        <v>94</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D78" t="s">
-        <v>176</v>
       </c>
       <c r="E78" s="3">
         <v>1</v>
@@ -3323,22 +3368,22 @@
         <v>6</v>
       </c>
       <c r="G78" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>176</v>
+      </c>
+      <c r="B79" t="s">
+        <v>93</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D79" t="s">
         <v>177</v>
       </c>
-      <c r="B79" t="s">
-        <v>94</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D79" t="s">
-        <v>178</v>
-      </c>
       <c r="E79" s="3">
         <v>1</v>
       </c>
@@ -3346,22 +3391,22 @@
         <v>7</v>
       </c>
       <c r="G79" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>178</v>
+      </c>
+      <c r="B80" t="s">
+        <v>93</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D80" t="s">
         <v>179</v>
       </c>
-      <c r="B80" t="s">
-        <v>94</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="D80" t="s">
-        <v>180</v>
-      </c>
       <c r="E80" s="3">
         <v>1</v>
       </c>
@@ -3369,22 +3414,22 @@
         <v>7</v>
       </c>
       <c r="G80" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>180</v>
+      </c>
+      <c r="B81" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D81" t="s">
         <v>181</v>
       </c>
-      <c r="B81" t="s">
-        <v>95</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D81" t="s">
-        <v>182</v>
-      </c>
       <c r="E81" s="3">
         <v>1</v>
       </c>
@@ -3392,21 +3437,21 @@
         <v>7</v>
       </c>
       <c r="G81" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>182</v>
+      </c>
+      <c r="B82" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D82" t="s">
         <v>183</v>
-      </c>
-      <c r="B82" t="s">
-        <v>96</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D82" t="s">
-        <v>184</v>
       </c>
       <c r="E82" s="3">
         <v>1</v>
@@ -3420,17 +3465,17 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>184</v>
+      </c>
+      <c r="B83" t="s">
+        <v>93</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D83" t="s">
         <v>185</v>
       </c>
-      <c r="B83" t="s">
-        <v>94</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="D83" t="s">
-        <v>186</v>
-      </c>
       <c r="E83" s="3">
         <v>1</v>
       </c>
@@ -3438,21 +3483,21 @@
         <v>7</v>
       </c>
       <c r="G83" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>186</v>
+      </c>
+      <c r="B84" t="s">
+        <v>93</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D84" t="s">
         <v>187</v>
-      </c>
-      <c r="B84" t="s">
-        <v>94</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="D84" t="s">
-        <v>188</v>
       </c>
       <c r="E84" s="3">
         <v>1</v>
@@ -3466,16 +3511,16 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>188</v>
+      </c>
+      <c r="B85" t="s">
+        <v>93</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D85" t="s">
         <v>189</v>
-      </c>
-      <c r="B85" t="s">
-        <v>94</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="D85" t="s">
-        <v>190</v>
       </c>
       <c r="E85" s="3">
         <v>1</v>
@@ -3489,16 +3534,16 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B86" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D86" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E86" s="3">
         <v>1</v>
@@ -3512,16 +3557,16 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>192</v>
+      </c>
+      <c r="B87" t="s">
+        <v>93</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D87" t="s">
         <v>193</v>
-      </c>
-      <c r="B87" t="s">
-        <v>94</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D87" t="s">
-        <v>194</v>
       </c>
       <c r="E87" s="3">
         <v>1</v>
@@ -3535,16 +3580,16 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>194</v>
+      </c>
+      <c r="B88" t="s">
+        <v>93</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D88" t="s">
         <v>195</v>
-      </c>
-      <c r="B88" t="s">
-        <v>94</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D88" t="s">
-        <v>196</v>
       </c>
       <c r="E88" s="3">
         <v>1</v>
@@ -3558,17 +3603,17 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>196</v>
+      </c>
+      <c r="B89" t="s">
+        <v>93</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D89" t="s">
         <v>197</v>
       </c>
-      <c r="B89" t="s">
-        <v>94</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="D89" t="s">
-        <v>198</v>
-      </c>
       <c r="E89" s="3">
         <v>1</v>
       </c>
@@ -3576,21 +3621,21 @@
         <v>7</v>
       </c>
       <c r="G89" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B90" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D90" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E90" s="3">
         <v>1</v>
@@ -3599,22 +3644,22 @@
         <v>7</v>
       </c>
       <c r="G90" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>199</v>
+      </c>
+      <c r="B91" t="s">
+        <v>93</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D91" t="s">
         <v>200</v>
       </c>
-      <c r="B91" t="s">
-        <v>94</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="D91" t="s">
-        <v>201</v>
-      </c>
       <c r="E91" s="3">
         <v>1</v>
       </c>
@@ -3622,22 +3667,22 @@
         <v>7</v>
       </c>
       <c r="G91" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>201</v>
+      </c>
+      <c r="B92" t="s">
+        <v>93</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D92" t="s">
         <v>202</v>
       </c>
-      <c r="B92" t="s">
-        <v>94</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D92" t="s">
-        <v>203</v>
-      </c>
       <c r="E92" s="3">
         <v>1</v>
       </c>
@@ -3645,38 +3690,38 @@
         <v>7</v>
       </c>
       <c r="G92" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>203</v>
+      </c>
+      <c r="B93" t="s">
+        <v>93</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B93" t="s">
-        <v>94</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="F93" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G93" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>205</v>
+      </c>
+      <c r="B94" t="s">
+        <v>95</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D94" t="s">
         <v>206</v>
-      </c>
-      <c r="B94" t="s">
-        <v>96</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D94" t="s">
-        <v>207</v>
       </c>
       <c r="E94" s="3">
         <v>1</v>
@@ -3690,17 +3735,17 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>207</v>
+      </c>
+      <c r="B95" t="s">
+        <v>93</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D95" t="s">
         <v>208</v>
       </c>
-      <c r="B95" t="s">
-        <v>94</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D95" t="s">
-        <v>209</v>
-      </c>
       <c r="E95" s="3">
         <v>1</v>
       </c>
@@ -3708,22 +3753,22 @@
         <v>7</v>
       </c>
       <c r="G95" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>209</v>
+      </c>
+      <c r="B96" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="D96" t="s">
         <v>210</v>
       </c>
-      <c r="B96" t="s">
-        <v>94</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="D96" t="s">
-        <v>211</v>
-      </c>
       <c r="E96" s="3">
         <v>1</v>
       </c>
@@ -3731,21 +3776,21 @@
         <v>7</v>
       </c>
       <c r="G96" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>211</v>
+      </c>
+      <c r="B97" t="s">
+        <v>93</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D97" t="s">
         <v>212</v>
-      </c>
-      <c r="B97" t="s">
-        <v>94</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D97" t="s">
-        <v>213</v>
       </c>
       <c r="E97" s="3">
         <v>1</v>
@@ -3759,17 +3804,17 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>213</v>
+      </c>
+      <c r="B98" t="s">
+        <v>93</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D98" t="s">
         <v>214</v>
       </c>
-      <c r="B98" t="s">
-        <v>94</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="D98" t="s">
-        <v>215</v>
-      </c>
       <c r="E98" s="3">
         <v>1</v>
       </c>
@@ -3777,22 +3822,22 @@
         <v>7</v>
       </c>
       <c r="G98" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>215</v>
+      </c>
+      <c r="B99" t="s">
+        <v>93</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D99" t="s">
         <v>216</v>
       </c>
-      <c r="B99" t="s">
-        <v>94</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="D99" t="s">
-        <v>217</v>
-      </c>
       <c r="E99" s="3">
         <v>1</v>
       </c>
@@ -3800,22 +3845,22 @@
         <v>7</v>
       </c>
       <c r="G99" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>316</v>
+      </c>
+      <c r="B100" t="s">
+        <v>93</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D100" t="s">
         <v>318</v>
       </c>
-      <c r="B100" t="s">
-        <v>94</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="D100" t="s">
-        <v>320</v>
-      </c>
       <c r="E100" s="3">
         <v>1</v>
       </c>
@@ -3823,21 +3868,21 @@
         <v>7</v>
       </c>
       <c r="G100" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>319</v>
+      </c>
+      <c r="B101" t="s">
+        <v>95</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B101" t="s">
-        <v>96</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>323</v>
-      </c>
       <c r="D101" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E101" s="3">
         <v>1</v>
@@ -3846,21 +3891,21 @@
         <v>7</v>
       </c>
       <c r="G101" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>322</v>
+      </c>
+      <c r="B102" t="s">
+        <v>95</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B102" t="s">
-        <v>96</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="D102" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E102" s="3">
         <v>1</v>
@@ -3874,16 +3919,16 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>325</v>
+      </c>
+      <c r="B103" t="s">
+        <v>93</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D103" t="s">
         <v>327</v>
-      </c>
-      <c r="B103" t="s">
-        <v>94</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D103" t="s">
-        <v>329</v>
       </c>
       <c r="E103" s="3">
         <v>1</v>
@@ -3897,17 +3942,17 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>328</v>
+      </c>
+      <c r="B104" t="s">
+        <v>95</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D104" t="s">
         <v>330</v>
       </c>
-      <c r="B104" t="s">
-        <v>96</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D104" t="s">
-        <v>332</v>
-      </c>
       <c r="E104" s="3">
         <v>1</v>
       </c>
@@ -3915,22 +3960,22 @@
         <v>7</v>
       </c>
       <c r="G104" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>331</v>
+      </c>
+      <c r="B105" t="s">
+        <v>93</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D105" t="s">
         <v>333</v>
       </c>
-      <c r="B105" t="s">
-        <v>94</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="D105" t="s">
-        <v>335</v>
-      </c>
       <c r="E105" s="3">
         <v>1</v>
       </c>
@@ -3938,21 +3983,21 @@
         <v>7</v>
       </c>
       <c r="G105" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>334</v>
+      </c>
+      <c r="B106" t="s">
+        <v>93</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D106" t="s">
         <v>336</v>
-      </c>
-      <c r="B106" t="s">
-        <v>94</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="D106" t="s">
-        <v>338</v>
       </c>
       <c r="E106" s="3">
         <v>1</v>
@@ -3961,44 +4006,44 @@
         <v>6</v>
       </c>
       <c r="G106" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>337</v>
+      </c>
+      <c r="B107" t="s">
+        <v>95</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D107" t="s">
         <v>339</v>
       </c>
-      <c r="B107" t="s">
-        <v>96</v>
-      </c>
-      <c r="C107" s="2" t="s">
+      <c r="E107" s="3">
+        <v>1</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G107" t="s">
         <v>340</v>
-      </c>
-      <c r="D107" t="s">
-        <v>341</v>
-      </c>
-      <c r="E107" s="3">
-        <v>1</v>
-      </c>
-      <c r="F107" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G107" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>341</v>
+      </c>
+      <c r="B108" t="s">
+        <v>95</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D108" t="s">
         <v>343</v>
-      </c>
-      <c r="B108" t="s">
-        <v>96</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="D108" t="s">
-        <v>345</v>
       </c>
       <c r="E108" s="3">
         <v>1</v>
@@ -4012,16 +4057,16 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>344</v>
+      </c>
+      <c r="B109" t="s">
+        <v>93</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D109" t="s">
         <v>346</v>
-      </c>
-      <c r="B109" t="s">
-        <v>94</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="D109" t="s">
-        <v>348</v>
       </c>
       <c r="E109" s="3">
         <v>1</v>
@@ -4031,6 +4076,121 @@
       </c>
       <c r="G109" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>347</v>
+      </c>
+      <c r="B110" t="s">
+        <v>94</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D110" t="s">
+        <v>349</v>
+      </c>
+      <c r="E110" s="3">
+        <v>1</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G110" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>350</v>
+      </c>
+      <c r="B111" t="s">
+        <v>93</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D111" t="s">
+        <v>352</v>
+      </c>
+      <c r="E111" s="3">
+        <v>1</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G111" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>353</v>
+      </c>
+      <c r="B112" t="s">
+        <v>93</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D112" t="s">
+        <v>355</v>
+      </c>
+      <c r="E112" s="3">
+        <v>1</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G112" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>356</v>
+      </c>
+      <c r="B113" t="s">
+        <v>93</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D113" t="s">
+        <v>358</v>
+      </c>
+      <c r="E113" s="3">
+        <v>1</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G113" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>360</v>
+      </c>
+      <c r="B114" t="s">
+        <v>94</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D114" t="s">
+        <v>361</v>
+      </c>
+      <c r="E114" s="3">
+        <v>1</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G114" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -4062,6 +4222,11 @@
     <hyperlink ref="C107" r:id="rId14" xr:uid="{43B1F1E3-061F-6F4F-9330-8E8D5B03E3E9}"/>
     <hyperlink ref="C108" r:id="rId15" xr:uid="{45971529-0C3A-314D-BB31-CCCDE4921AB5}"/>
     <hyperlink ref="C109" r:id="rId16" xr:uid="{C3A446B8-F146-1D4D-8A9F-EF8B8ACAB0AD}"/>
+    <hyperlink ref="C110" r:id="rId17" xr:uid="{BDEEFBE0-AC99-4446-B799-0EEEC2196B21}"/>
+    <hyperlink ref="C111" r:id="rId18" xr:uid="{8AB60306-10F0-B24B-9D65-CB3CAEB6CED8}"/>
+    <hyperlink ref="C112" r:id="rId19" xr:uid="{79D4402B-D589-3B47-B936-740FD74DD0E1}"/>
+    <hyperlink ref="C113" r:id="rId20" xr:uid="{7C191B5E-EC2C-394E-AC17-A9D1822F5FCA}"/>
+    <hyperlink ref="C24" r:id="rId21" xr:uid="{184BBE5D-CFF2-934F-96FB-2016C393E280}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 4/26
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B4AFBC-AF50-E642-92D2-27F689FB07F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030CF819-5E4F-D14C-A74A-A6CF9A6BD79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="367">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1128,6 +1128,15 @@
   </si>
   <si>
     <t>Top down DP, keep dp[10][n+1], just go through each neighbor for each index till n one, store and update result</t>
+  </si>
+  <si>
+    <t>Longest Ideal Subsequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-ideal-subsequence/submissions/1242916834/</t>
+  </si>
+  <si>
+    <t>Store 26-len array of letters with their best length, loop over all letters each time and track best length and update global max to local max</t>
   </si>
 </sst>
 </file>
@@ -1554,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:J114"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4191,6 +4200,29 @@
       </c>
       <c r="G114" t="s">
         <v>340</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>364</v>
+      </c>
+      <c r="B115" t="s">
+        <v>93</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="D115" t="s">
+        <v>366</v>
+      </c>
+      <c r="E115" s="3">
+        <v>1</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G115" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -4227,6 +4259,7 @@
     <hyperlink ref="C112" r:id="rId19" xr:uid="{79D4402B-D589-3B47-B936-740FD74DD0E1}"/>
     <hyperlink ref="C113" r:id="rId20" xr:uid="{7C191B5E-EC2C-394E-AC17-A9D1822F5FCA}"/>
     <hyperlink ref="C24" r:id="rId21" xr:uid="{184BBE5D-CFF2-934F-96FB-2016C393E280}"/>
+    <hyperlink ref="C115" r:id="rId22" xr:uid="{1C1629E6-342E-5D4E-9B39-CB46C4F6BEA3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 5/5
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030CF819-5E4F-D14C-A74A-A6CF9A6BD79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ECF0D8-4403-4D47-9D95-C39B538296AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="370">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1137,6 +1137,15 @@
   </si>
   <si>
     <t>Store 26-len array of letters with their best length, loop over all letters each time and track best length and update global max to local max</t>
+  </si>
+  <si>
+    <t>Boats to Save People</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/boats-to-save-people/submissions/1250548443/</t>
+  </si>
+  <si>
+    <t>Greedy approach, sort then l=0, r=n-1, if sum fits in limit you fit both, otherwise move r down</t>
   </si>
 </sst>
 </file>
@@ -1563,10 +1572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4223,6 +4232,29 @@
       </c>
       <c r="G115" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>367</v>
+      </c>
+      <c r="B116" t="s">
+        <v>93</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D116" t="s">
+        <v>369</v>
+      </c>
+      <c r="E116" s="3">
+        <v>1</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G116" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4260,6 +4292,7 @@
     <hyperlink ref="C113" r:id="rId20" xr:uid="{7C191B5E-EC2C-394E-AC17-A9D1822F5FCA}"/>
     <hyperlink ref="C24" r:id="rId21" xr:uid="{184BBE5D-CFF2-934F-96FB-2016C393E280}"/>
     <hyperlink ref="C115" r:id="rId22" xr:uid="{1C1629E6-342E-5D4E-9B39-CB46C4F6BEA3}"/>
+    <hyperlink ref="C116" r:id="rId23" xr:uid="{F0032CD0-D24F-4C42-AEB0-07F228E97F16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 5/7
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36ECF0D8-4403-4D47-9D95-C39B538296AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17A3B6E-EEE5-DB49-A6FD-C5539FBE5535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="389">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1121,9 +1121,6 @@
     <t>Longest Valid Parentheses</t>
   </si>
   <si>
-    <t>Store array, whenever you encounter valid paren pairs, convert corr. Index in arr to same symbol, find longest contiguous occurrences of symbol</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/knight-dialer/submissions/1241442723/</t>
   </si>
   <si>
@@ -1146,6 +1143,66 @@
   </si>
   <si>
     <t>Greedy approach, sort then l=0, r=n-1, if sum fits in limit you fit both, otherwise move r down</t>
+  </si>
+  <si>
+    <t>Remove Nodes from Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-nodes-from-linked-list/submissions/1250581294/</t>
+  </si>
+  <si>
+    <t>Monotonic stack, just set invalid nodes to val -1 when they break decreasing condition</t>
+  </si>
+  <si>
+    <t>Store array, whenever you encounter valid paren pairs, convert corr. index in arr to same symbol, find longest contiguous occurrences of symbol</t>
+  </si>
+  <si>
+    <t>Trapping Rain Water</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/trapping-rain-water/submissions/1251276397/</t>
+  </si>
+  <si>
+    <t>Find max on left and max on right at each position, use to calculate rain stored</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Can optimize to two pointer, just do l=0, r=n-1, and keep two maxes, and move whatever's lesser, update your maxes and total rain</t>
+  </si>
+  <si>
+    <t>Minimum Equal Sum of the Two Arrays After Replacing Zeroes</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-equal-sum-of-two-arrays-after-replacing-zeros/submissions/1251369742/</t>
+  </si>
+  <si>
+    <t>Count ones and zeros, if both have zeros always valid, otherwise check if setting 1 for all 0s makes it too big in both cases</t>
+  </si>
+  <si>
+    <t>Longest Non Decreasing Subarray From Two Arrays</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-non-decreasing-subarray-from-two-arrays/submissions/1251492568/</t>
+  </si>
+  <si>
+    <t>Two-state dp arr(n), longest subarray till that point but reset to 1 when needed</t>
+  </si>
+  <si>
+    <t>Can optimize to not use DP array since subarrays are contiguous</t>
+  </si>
+  <si>
+    <t>Minimum Knight Moves</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-knight-moves/submissions/1252197254/</t>
+  </si>
+  <si>
+    <t>BFS, keep track of visited cells, queue should have x, y, current move num, return moves on first correct point</t>
+  </si>
+  <si>
+    <t>Can optimize to not use BFS and solve it in closed form, there's a mathematical O(1) solution</t>
   </si>
 </sst>
 </file>
@@ -1223,7 +1280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1235,6 +1292,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1572,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:J116"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1587,10 +1650,11 @@
     <col min="5" max="5" width="10.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="43.33203125" customWidth="1"/>
     <col min="10" max="10" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1612,15 +1676,17 @@
       <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1642,14 +1708,15 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="10"/>
+      <c r="J2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1671,14 +1738,15 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="H3" s="10"/>
+      <c r="J3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1700,14 +1768,15 @@
       <c r="G4" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="10"/>
+      <c r="J4" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1729,8 +1798,9 @@
       <c r="G5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1752,8 +1822,9 @@
       <c r="G6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1775,8 +1846,9 @@
       <c r="G7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1798,8 +1870,9 @@
       <c r="G8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1821,8 +1894,9 @@
       <c r="G9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1844,8 +1918,9 @@
       <c r="G10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1867,8 +1942,9 @@
       <c r="G11" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1890,8 +1966,9 @@
       <c r="G12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1911,8 +1988,9 @@
       <c r="G13" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1934,8 +2012,9 @@
       <c r="G14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1957,8 +2036,9 @@
       <c r="G15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1980,8 +2060,9 @@
       <c r="G16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2003,8 +2084,9 @@
       <c r="G17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2026,8 +2108,9 @@
       <c r="G18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -2049,8 +2132,9 @@
       <c r="G19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2072,8 +2156,9 @@
       <c r="G20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -2095,8 +2180,9 @@
       <c r="G21" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2118,8 +2204,9 @@
       <c r="G22" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2141,8 +2228,9 @@
       <c r="G23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2150,10 +2238,10 @@
         <v>93</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D24" t="s">
         <v>362</v>
-      </c>
-      <c r="D24" t="s">
-        <v>363</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -2164,8 +2252,9 @@
       <c r="G24" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -2187,8 +2276,9 @@
       <c r="G25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -2210,8 +2300,9 @@
       <c r="G26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -2233,8 +2324,9 @@
       <c r="G27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2256,8 +2348,9 @@
       <c r="G28" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -2279,8 +2372,9 @@
       <c r="G29" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -2302,8 +2396,9 @@
       <c r="G30" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -2325,8 +2420,9 @@
       <c r="G31" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -2348,8 +2444,9 @@
       <c r="G32" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -2371,8 +2468,9 @@
       <c r="G33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2394,8 +2492,9 @@
       <c r="G34" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2417,8 +2516,9 @@
       <c r="G35" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -2440,8 +2540,9 @@
       <c r="G36" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -2463,8 +2564,9 @@
       <c r="G37" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -2486,8 +2588,9 @@
       <c r="G38" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -2509,8 +2612,9 @@
       <c r="G39" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -2532,8 +2636,9 @@
       <c r="G40" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -2555,8 +2660,9 @@
       <c r="G41" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -2578,8 +2684,9 @@
       <c r="G42" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" s="10"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -2601,8 +2708,9 @@
       <c r="G43" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>101</v>
       </c>
@@ -2624,8 +2732,9 @@
       <c r="G44" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" s="10"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>103</v>
       </c>
@@ -2647,8 +2756,9 @@
       <c r="G45" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" s="10"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>106</v>
       </c>
@@ -2670,8 +2780,9 @@
       <c r="G46" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" s="10"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>108</v>
       </c>
@@ -2693,8 +2804,9 @@
       <c r="G47" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" s="10"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>110</v>
       </c>
@@ -2716,8 +2828,9 @@
       <c r="G48" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="10"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -2739,8 +2852,9 @@
       <c r="G49" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" s="10"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -2762,8 +2876,9 @@
       <c r="G50" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="10"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>119</v>
       </c>
@@ -2785,8 +2900,9 @@
       <c r="G51" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>118</v>
       </c>
@@ -2805,8 +2921,9 @@
       <c r="G52" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="10"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>122</v>
       </c>
@@ -2828,8 +2945,9 @@
       <c r="G53" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="10"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>123</v>
       </c>
@@ -2848,8 +2966,9 @@
       <c r="G54" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="10"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>125</v>
       </c>
@@ -2871,8 +2990,9 @@
       <c r="G55" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="10"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>127</v>
       </c>
@@ -2894,8 +3014,9 @@
       <c r="G56" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="10"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>129</v>
       </c>
@@ -2917,8 +3038,9 @@
       <c r="G57" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="10"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>132</v>
       </c>
@@ -2940,8 +3062,9 @@
       <c r="G58" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="10"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>134</v>
       </c>
@@ -2963,8 +3086,9 @@
       <c r="G59" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H59" s="10"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>137</v>
       </c>
@@ -2986,8 +3110,9 @@
       <c r="G60" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H60" s="10"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -3009,8 +3134,9 @@
       <c r="G61" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H61" s="10"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>141</v>
       </c>
@@ -3032,8 +3158,9 @@
       <c r="G62" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H62" s="10"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>143</v>
       </c>
@@ -3055,8 +3182,9 @@
       <c r="G63" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="10"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -3078,8 +3206,9 @@
       <c r="G64" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H64" s="10"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -3101,8 +3230,9 @@
       <c r="G65" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H65" s="10"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -3124,8 +3254,9 @@
       <c r="G66" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66" s="10"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>151</v>
       </c>
@@ -3141,8 +3272,9 @@
       <c r="G67" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>154</v>
       </c>
@@ -3158,8 +3290,9 @@
       <c r="G68" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H68" s="10"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>155</v>
       </c>
@@ -3181,8 +3314,9 @@
       <c r="G69" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H69" s="10"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>157</v>
       </c>
@@ -3204,8 +3338,9 @@
       <c r="G70" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H70" s="10"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>159</v>
       </c>
@@ -3227,8 +3362,9 @@
       <c r="G71" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H71" s="10"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>162</v>
       </c>
@@ -3250,8 +3386,9 @@
       <c r="G72" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H72" s="10"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>164</v>
       </c>
@@ -3273,8 +3410,9 @@
       <c r="G73" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H73" s="10"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>166</v>
       </c>
@@ -3296,8 +3434,9 @@
       <c r="G74" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H74" s="10"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>168</v>
       </c>
@@ -3319,8 +3458,9 @@
       <c r="G75" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H75" s="10"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>169</v>
       </c>
@@ -3342,8 +3482,9 @@
       <c r="G76" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H76" s="10"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>172</v>
       </c>
@@ -3365,8 +3506,9 @@
       <c r="G77" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H77" s="10"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>174</v>
       </c>
@@ -3388,8 +3530,9 @@
       <c r="G78" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H78" s="10"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>176</v>
       </c>
@@ -3411,8 +3554,9 @@
       <c r="G79" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H79" s="10"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>178</v>
       </c>
@@ -3434,8 +3578,9 @@
       <c r="G80" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80" s="10"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>180</v>
       </c>
@@ -3457,8 +3602,9 @@
       <c r="G81" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H81" s="10"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -3480,8 +3626,9 @@
       <c r="G82" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H82" s="10"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>184</v>
       </c>
@@ -3503,8 +3650,9 @@
       <c r="G83" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H83" s="10"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>186</v>
       </c>
@@ -3526,8 +3674,9 @@
       <c r="G84" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H84" s="10"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>188</v>
       </c>
@@ -3549,8 +3698,9 @@
       <c r="G85" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H85" s="10"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>191</v>
       </c>
@@ -3572,8 +3722,9 @@
       <c r="G86" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H86" s="10"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>192</v>
       </c>
@@ -3595,8 +3746,9 @@
       <c r="G87" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H87" s="10"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>194</v>
       </c>
@@ -3618,8 +3770,9 @@
       <c r="G88" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H88" s="10"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -3641,8 +3794,9 @@
       <c r="G89" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H89" s="10"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>198</v>
       </c>
@@ -3664,8 +3818,9 @@
       <c r="G90" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H90" s="10"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>199</v>
       </c>
@@ -3687,8 +3842,9 @@
       <c r="G91" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H91" s="10"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>201</v>
       </c>
@@ -3710,8 +3866,9 @@
       <c r="G92" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92" s="10"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>203</v>
       </c>
@@ -3727,8 +3884,9 @@
       <c r="G93" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93" s="10"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>205</v>
       </c>
@@ -3750,8 +3908,9 @@
       <c r="G94" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94" s="10"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>207</v>
       </c>
@@ -3773,8 +3932,9 @@
       <c r="G95" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95" s="10"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>209</v>
       </c>
@@ -3796,8 +3956,9 @@
       <c r="G96" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H96" s="10"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>211</v>
       </c>
@@ -3819,8 +3980,9 @@
       <c r="G97" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H97" s="10"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>213</v>
       </c>
@@ -3842,8 +4004,9 @@
       <c r="G98" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H98" s="10"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>215</v>
       </c>
@@ -3865,8 +4028,9 @@
       <c r="G99" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H99" s="10"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>316</v>
       </c>
@@ -3888,8 +4052,9 @@
       <c r="G100" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H100" s="10"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>319</v>
       </c>
@@ -3911,8 +4076,9 @@
       <c r="G101" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H101" s="10"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>322</v>
       </c>
@@ -3934,8 +4100,9 @@
       <c r="G102" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102" s="10"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>325</v>
       </c>
@@ -3957,8 +4124,9 @@
       <c r="G103" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103" s="10"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>328</v>
       </c>
@@ -3980,8 +4148,9 @@
       <c r="G104" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H104" s="10"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>331</v>
       </c>
@@ -4003,8 +4172,9 @@
       <c r="G105" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H105" s="10"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>334</v>
       </c>
@@ -4026,8 +4196,9 @@
       <c r="G106" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H106" s="10"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>337</v>
       </c>
@@ -4049,8 +4220,9 @@
       <c r="G107" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H107" s="10"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>341</v>
       </c>
@@ -4072,8 +4244,9 @@
       <c r="G108" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H108" s="10"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>344</v>
       </c>
@@ -4095,8 +4268,9 @@
       <c r="G109" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H109" s="10"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>347</v>
       </c>
@@ -4118,8 +4292,9 @@
       <c r="G110" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H110" s="10"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>350</v>
       </c>
@@ -4141,8 +4316,9 @@
       <c r="G111" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H111" s="10"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>353</v>
       </c>
@@ -4164,8 +4340,9 @@
       <c r="G112" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H112" s="10"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>356</v>
       </c>
@@ -4187,8 +4364,9 @@
       <c r="G113" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H113" s="10"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>360</v>
       </c>
@@ -4199,7 +4377,7 @@
         <v>359</v>
       </c>
       <c r="D114" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
       <c r="E114" s="3">
         <v>1</v>
@@ -4210,19 +4388,20 @@
       <c r="G114" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H114" s="10"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>363</v>
+      </c>
+      <c r="B115" t="s">
+        <v>93</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B115" t="s">
-        <v>93</v>
-      </c>
-      <c r="C115" s="2" t="s">
+      <c r="D115" t="s">
         <v>365</v>
-      </c>
-      <c r="D115" t="s">
-        <v>366</v>
       </c>
       <c r="E115" s="3">
         <v>1</v>
@@ -4233,19 +4412,20 @@
       <c r="G115" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H115" s="10"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>366</v>
+      </c>
+      <c r="B116" t="s">
+        <v>93</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B116" t="s">
-        <v>93</v>
-      </c>
-      <c r="C116" s="2" t="s">
+      <c r="D116" t="s">
         <v>368</v>
-      </c>
-      <c r="D116" t="s">
-        <v>369</v>
       </c>
       <c r="E116" s="3">
         <v>1</v>
@@ -4255,6 +4435,132 @@
       </c>
       <c r="G116" t="s">
         <v>120</v>
+      </c>
+      <c r="H116" s="10"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>369</v>
+      </c>
+      <c r="B117" t="s">
+        <v>93</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D117" t="s">
+        <v>371</v>
+      </c>
+      <c r="E117" s="3">
+        <v>1</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G117" t="s">
+        <v>340</v>
+      </c>
+      <c r="H117" s="10"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>373</v>
+      </c>
+      <c r="B118" t="s">
+        <v>94</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D118" t="s">
+        <v>375</v>
+      </c>
+      <c r="E118" s="3">
+        <v>1</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G118" t="s">
+        <v>107</v>
+      </c>
+      <c r="H118" s="10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>378</v>
+      </c>
+      <c r="B119" t="s">
+        <v>93</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="D119" t="s">
+        <v>380</v>
+      </c>
+      <c r="E119" s="3">
+        <v>1</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G119" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>381</v>
+      </c>
+      <c r="B120" t="s">
+        <v>93</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D120" t="s">
+        <v>383</v>
+      </c>
+      <c r="E120" s="3">
+        <v>1</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G120" t="s">
+        <v>107</v>
+      </c>
+      <c r="H120" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>385</v>
+      </c>
+      <c r="B121" t="s">
+        <v>93</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D121" t="s">
+        <v>387</v>
+      </c>
+      <c r="E121" s="3">
+        <v>1</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G121" t="s">
+        <v>16</v>
+      </c>
+      <c r="H121" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -4293,6 +4599,12 @@
     <hyperlink ref="C24" r:id="rId21" xr:uid="{184BBE5D-CFF2-934F-96FB-2016C393E280}"/>
     <hyperlink ref="C115" r:id="rId22" xr:uid="{1C1629E6-342E-5D4E-9B39-CB46C4F6BEA3}"/>
     <hyperlink ref="C116" r:id="rId23" xr:uid="{F0032CD0-D24F-4C42-AEB0-07F228E97F16}"/>
+    <hyperlink ref="C117" r:id="rId24" xr:uid="{06E01083-ACC7-5E44-A501-92E4F54880CE}"/>
+    <hyperlink ref="C114" r:id="rId25" xr:uid="{B5F8E582-5EC3-824D-958A-9AB4E0DA09D9}"/>
+    <hyperlink ref="C118" r:id="rId26" xr:uid="{11FD39F8-9BF0-B44A-B5AF-DEB2AF4AC482}"/>
+    <hyperlink ref="C119" r:id="rId27" xr:uid="{24EEE1F0-A430-6947-B016-2DBF7687E37E}"/>
+    <hyperlink ref="C120" r:id="rId28" xr:uid="{04F7BED6-485B-9D41-94CE-8B7EA329AF28}"/>
+    <hyperlink ref="C121" r:id="rId29" xr:uid="{34281855-A30F-5044-8368-DE083C5FB097}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 5/12
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17A3B6E-EEE5-DB49-A6FD-C5539FBE5535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520A61C3-2A6B-9D41-A8A1-6321E4EFE4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="413">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1203,6 +1203,78 @@
   </si>
   <si>
     <t>Can optimize to not use BFS and solve it in closed form, there's a mathematical O(1) solution</t>
+  </si>
+  <si>
+    <t>Relative Ranks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greedy </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/relative-ranks/submissions/1253038484/</t>
+  </si>
+  <si>
+    <t>Sort the array by greatest to lowest scores, assign places based on that</t>
+  </si>
+  <si>
+    <t>Delete and Earn</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/delete-and-earn/submissions/1253101656/</t>
+  </si>
+  <si>
+    <t>Dp[1…maxnum], dp[i] = max(current sum and dp[i-2], dp[i-1]), similar recurrence to house robbers</t>
+  </si>
+  <si>
+    <t>Can optimize to O(1) space since you only need dp[i-1] and dp[i-2] (just like House Robbers)</t>
+  </si>
+  <si>
+    <t>Connor was goating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximize Happiness of Selected Children </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximize-happiness-of-selected-children/submissions/1253880225/</t>
+  </si>
+  <si>
+    <t>Sort list, keep taking maximum and subtract offset, only add elements if (num - offset) &gt; 0</t>
+  </si>
+  <si>
+    <t>K-th Smallest Prime Fraction</t>
+  </si>
+  <si>
+    <t>Binary search on the answer, go through and find count of fractions greater than current value (starting at .5, updating as needed), when it equals k you return</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/k-th-smallest-prime-fraction/submissions/1254817739/</t>
+  </si>
+  <si>
+    <t>Need to study more binary searching on the answer</t>
+  </si>
+  <si>
+    <t>LFU Cache</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lfu-cache/submissions/1255395985/</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>C++ doesn't have LinkedHashSet, but could've used that, and weighted stuff by freq-value</t>
+  </si>
+  <si>
+    <t>Implement LRU Cache, keep map of usage-&gt;LRU, keys-&gt;usage, support operations in O(1) and maintain minimum usage level</t>
+  </si>
+  <si>
+    <t>Evaluate Division</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/evaluate-division/submissions/1256068944/</t>
+  </si>
+  <si>
+    <t>Convert to graph problem where nodes have in/out edges, traverse graph and keep a running product</t>
   </si>
 </sst>
 </file>
@@ -1635,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:K121"/>
+  <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="158" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4561,6 +4633,156 @@
       </c>
       <c r="H121" t="s">
         <v>388</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>389</v>
+      </c>
+      <c r="B122" t="s">
+        <v>95</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D122" t="s">
+        <v>392</v>
+      </c>
+      <c r="E122" s="3">
+        <v>1</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G122" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>393</v>
+      </c>
+      <c r="B123" t="s">
+        <v>93</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D123" t="s">
+        <v>395</v>
+      </c>
+      <c r="E123" s="3">
+        <v>1</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G123" t="s">
+        <v>107</v>
+      </c>
+      <c r="H123" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>398</v>
+      </c>
+      <c r="B124" t="s">
+        <v>93</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D124" t="s">
+        <v>400</v>
+      </c>
+      <c r="E124" s="3">
+        <v>1</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G124" t="s">
+        <v>13</v>
+      </c>
+      <c r="H124" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>401</v>
+      </c>
+      <c r="B125" t="s">
+        <v>93</v>
+      </c>
+      <c r="C125" t="s">
+        <v>403</v>
+      </c>
+      <c r="D125" t="s">
+        <v>402</v>
+      </c>
+      <c r="E125" s="3">
+        <v>1</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G125" t="s">
+        <v>111</v>
+      </c>
+      <c r="H125" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>405</v>
+      </c>
+      <c r="B126" t="s">
+        <v>94</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D126" t="s">
+        <v>409</v>
+      </c>
+      <c r="E126" s="3">
+        <v>1</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G126" t="s">
+        <v>407</v>
+      </c>
+      <c r="H126" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>410</v>
+      </c>
+      <c r="B127" t="s">
+        <v>93</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D127" t="s">
+        <v>412</v>
+      </c>
+      <c r="E127" s="3">
+        <v>1</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G127" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -4605,6 +4827,11 @@
     <hyperlink ref="C119" r:id="rId27" xr:uid="{24EEE1F0-A430-6947-B016-2DBF7687E37E}"/>
     <hyperlink ref="C120" r:id="rId28" xr:uid="{04F7BED6-485B-9D41-94CE-8B7EA329AF28}"/>
     <hyperlink ref="C121" r:id="rId29" xr:uid="{34281855-A30F-5044-8368-DE083C5FB097}"/>
+    <hyperlink ref="C122" r:id="rId30" xr:uid="{CFAADF87-ACD5-AA48-ADAD-9B1318DE7EF1}"/>
+    <hyperlink ref="C123" r:id="rId31" xr:uid="{A8F77FE2-9935-6245-B800-14B8EB4130FD}"/>
+    <hyperlink ref="C124" r:id="rId32" xr:uid="{5D7D207C-63CB-B34A-8C47-10ACDCF4AD13}"/>
+    <hyperlink ref="C126" r:id="rId33" xr:uid="{36510AE8-E179-C344-AEE0-756664F7D85B}"/>
+    <hyperlink ref="C127" r:id="rId34" xr:uid="{05A9F90F-93D2-1647-9F6D-15BEF1CAB826}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 5/23
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520A61C3-2A6B-9D41-A8A1-6321E4EFE4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D97793-DA81-3C43-8F00-CD6B4825059C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="414">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1275,6 +1275,9 @@
   </si>
   <si>
     <t>Convert to graph problem where nodes have in/out edges, traverse graph and keep a running product</t>
+  </si>
+  <si>
+    <t>Search Suggestions System</t>
   </si>
 </sst>
 </file>
@@ -1707,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:K127"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A114" zoomScale="158" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128"/>
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4783,6 +4786,14 @@
       </c>
       <c r="G127" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>413</v>
+      </c>
+      <c r="B128" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LC Tracking - 5/26
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D97793-DA81-3C43-8F00-CD6B4825059C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9B185A-8A37-C24C-851F-84440DFF9411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="424">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1278,6 +1278,36 @@
   </si>
   <si>
     <t>Search Suggestions System</t>
+  </si>
+  <si>
+    <t>Longest Increasing Path in a Matrix</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-increasing-path-in-a-matrix/submissions/1265462394/</t>
+  </si>
+  <si>
+    <t>DFS on every cell, check 4 directions, have DP array that stores best path starting at i,j</t>
+  </si>
+  <si>
+    <t>Sudoku Solver</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sudoku-solver/submissions/1266101936/</t>
+  </si>
+  <si>
+    <t>Trie</t>
+  </si>
+  <si>
+    <t>Write helpers to find candidates at some position, recurse on all candidates, false if you don't finish board or candidates is empty</t>
+  </si>
+  <si>
+    <t>Word Break</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-break/submissions/1267069381/</t>
+  </si>
+  <si>
+    <t>1D dp[n], at each index loop over all words in list and if substring is equal to a word, set dp[i] to dp[i - word_size] (that position could be valid)</t>
   </si>
 </sst>
 </file>
@@ -1710,10 +1740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:K128"/>
+  <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="158" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="158" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4794,6 +4824,81 @@
       </c>
       <c r="B128" t="s">
         <v>93</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G128" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>414</v>
+      </c>
+      <c r="B129" t="s">
+        <v>94</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D129" t="s">
+        <v>416</v>
+      </c>
+      <c r="E129" s="3">
+        <v>1</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G129" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>417</v>
+      </c>
+      <c r="B130" t="s">
+        <v>94</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D130" t="s">
+        <v>420</v>
+      </c>
+      <c r="E130" s="3">
+        <v>1</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G130" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>421</v>
+      </c>
+      <c r="B131" t="s">
+        <v>93</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D131" t="s">
+        <v>423</v>
+      </c>
+      <c r="E131" s="3">
+        <v>1</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G131" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -4843,6 +4948,9 @@
     <hyperlink ref="C124" r:id="rId32" xr:uid="{5D7D207C-63CB-B34A-8C47-10ACDCF4AD13}"/>
     <hyperlink ref="C126" r:id="rId33" xr:uid="{36510AE8-E179-C344-AEE0-756664F7D85B}"/>
     <hyperlink ref="C127" r:id="rId34" xr:uid="{05A9F90F-93D2-1647-9F6D-15BEF1CAB826}"/>
+    <hyperlink ref="C129" r:id="rId35" xr:uid="{AD64BEE2-4BAC-5F4D-8637-08964EE06892}"/>
+    <hyperlink ref="C130" r:id="rId36" xr:uid="{8569C66F-9138-564F-BBAA-822EB5B6ECD7}"/>
+    <hyperlink ref="C131" r:id="rId37" xr:uid="{0170280A-8604-2349-96CF-6106B1A60C41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 5/29
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9B185A-8A37-C24C-851F-84440DFF9411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0E910F-7499-1B4E-928F-CCA693C22AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="430">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1308,6 +1308,24 @@
   </si>
   <si>
     <t>1D dp[n], at each index loop over all words in list and if substring is equal to a word, set dp[i] to dp[i - word_size] (that position could be valid)</t>
+  </si>
+  <si>
+    <t>Get Equal Substrings Within Budget</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/get-equal-substrings-within-budget/submissions/1270610236/</t>
+  </si>
+  <si>
+    <t>Keep track of longest valid substring window by subtracting from maxCost when r++ and adding back to maxCost when l++</t>
+  </si>
+  <si>
+    <t>Number of Good Binary Substrings</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-good-binary-strings/submissions/1271188455/</t>
+  </si>
+  <si>
+    <t>1D dp, increment dp[i] by dp[i - oneGroup] and by dp[i - zeroGroup], add result within min/max window</t>
   </si>
 </sst>
 </file>
@@ -1740,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:K131"/>
+  <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="158" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D132" sqref="D132"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4898,6 +4916,52 @@
         <v>7</v>
       </c>
       <c r="G131" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>424</v>
+      </c>
+      <c r="B132" t="s">
+        <v>93</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D132" t="s">
+        <v>426</v>
+      </c>
+      <c r="E132" s="3">
+        <v>1</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G132" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>427</v>
+      </c>
+      <c r="B133" t="s">
+        <v>93</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D133" t="s">
+        <v>429</v>
+      </c>
+      <c r="E133" s="3">
+        <v>1</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G133" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4951,6 +5015,8 @@
     <hyperlink ref="C129" r:id="rId35" xr:uid="{AD64BEE2-4BAC-5F4D-8637-08964EE06892}"/>
     <hyperlink ref="C130" r:id="rId36" xr:uid="{8569C66F-9138-564F-BBAA-822EB5B6ECD7}"/>
     <hyperlink ref="C131" r:id="rId37" xr:uid="{0170280A-8604-2349-96CF-6106B1A60C41}"/>
+    <hyperlink ref="C132" r:id="rId38" xr:uid="{97372385-9B05-7241-B1E1-A72AED3F4C48}"/>
+    <hyperlink ref="C133" r:id="rId39" xr:uid="{A9A95ABE-F190-354F-A0A6-2CBC2C3C8502}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 5/30
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0E910F-7499-1B4E-928F-CCA693C22AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA93262-EA9F-1745-BD38-F9FFE425ABC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="441">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1326,6 +1326,39 @@
   </si>
   <si>
     <t>1D dp, increment dp[i] by dp[i - oneGroup] and by dp[i - zeroGroup], add result within min/max window</t>
+  </si>
+  <si>
+    <t>Number of Steps to Reduce a Number in a Binary Representation to One</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-steps-to-reduce-a-number-in-binary-representation-to-one/submissions/1271224386/</t>
+  </si>
+  <si>
+    <t>Create function for adding by one, once you're a power of two end loop and add string length</t>
+  </si>
+  <si>
+    <t>Count Triplets That Can Form Two Arrays of Equal Xor</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-triplets-that-can-form-two-arrays-of-equal-xor/submissions/1272435485/</t>
+  </si>
+  <si>
+    <t>Simulation, just have three nested loops and check all possible triplets for equality</t>
+  </si>
+  <si>
+    <t>Can solve smarter by keeping track of carry for adding and continually halving it</t>
+  </si>
+  <si>
+    <t>Can do an easy n^2 version by keeping a prefix array</t>
+  </si>
+  <si>
+    <t>Binary Tree Vertical Order Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-vertical-order-traversal/submissions/1272801337/</t>
+  </si>
+  <si>
+    <t>In order traversal but keep track of offset for sorting, and depth for stable sorting within levels</t>
   </si>
 </sst>
 </file>
@@ -1758,15 +1791,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:K133"/>
+  <dimension ref="A1:K136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54" customWidth="1"/>
+    <col min="1" max="1" width="41.6640625" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
@@ -4850,7 +4883,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>414</v>
       </c>
@@ -4873,7 +4906,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>417</v>
       </c>
@@ -4896,7 +4929,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>421</v>
       </c>
@@ -4919,7 +4952,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>424</v>
       </c>
@@ -4942,7 +4975,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>427</v>
       </c>
@@ -4963,6 +4996,81 @@
       </c>
       <c r="G133" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>430</v>
+      </c>
+      <c r="B134" t="s">
+        <v>93</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D134" t="s">
+        <v>432</v>
+      </c>
+      <c r="E134" s="3">
+        <v>1</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G134" t="s">
+        <v>49</v>
+      </c>
+      <c r="H134" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>433</v>
+      </c>
+      <c r="B135" t="s">
+        <v>93</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D135" t="s">
+        <v>435</v>
+      </c>
+      <c r="E135" s="3">
+        <v>1</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G135" t="s">
+        <v>49</v>
+      </c>
+      <c r="H135" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>438</v>
+      </c>
+      <c r="B136" t="s">
+        <v>93</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D136" t="s">
+        <v>440</v>
+      </c>
+      <c r="E136" s="3">
+        <v>1</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G136" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -5017,6 +5125,9 @@
     <hyperlink ref="C131" r:id="rId37" xr:uid="{0170280A-8604-2349-96CF-6106B1A60C41}"/>
     <hyperlink ref="C132" r:id="rId38" xr:uid="{97372385-9B05-7241-B1E1-A72AED3F4C48}"/>
     <hyperlink ref="C133" r:id="rId39" xr:uid="{A9A95ABE-F190-354F-A0A6-2CBC2C3C8502}"/>
+    <hyperlink ref="C134" r:id="rId40" xr:uid="{E400A34D-7519-274B-8AA6-BDC1F8381CE4}"/>
+    <hyperlink ref="C135" r:id="rId41" xr:uid="{F8A0824E-0D06-5848-BBB1-1B4ABD266BCA}"/>
+    <hyperlink ref="C136" r:id="rId42" xr:uid="{3806FC75-E461-1C40-AA11-26F63CE8E0A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 6/5
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA93262-EA9F-1745-BD38-F9FFE425ABC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEFE75C-79F2-1A43-B62C-638B18C62D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="493">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1359,6 +1359,162 @@
   </si>
   <si>
     <t>In order traversal but keep track of offset for sorting, and depth for stable sorting within levels</t>
+  </si>
+  <si>
+    <t>Valid Word Abbreviations</t>
+  </si>
+  <si>
+    <t>Weirdly annoying for an easy, crazy amount of edge cases</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-word-abbreviation/submissions/1272920303/</t>
+  </si>
+  <si>
+    <t>Loop through abbreviation and check if numbers are accurate, account for all kinds of edge cases</t>
+  </si>
+  <si>
+    <t>Single Number III</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/single-number-iii/submissions/1272951576/</t>
+  </si>
+  <si>
+    <t>Go through nums to get unique bit between target numbers, use that to separate into groups with bitmask and xor again to find first/second target</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor of a Binary Tree III</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree-iii/submissions/1273606341/</t>
+  </si>
+  <si>
+    <t>Get list of {parent, depth} for both nodes, iterate through both lists with two pointers and keep best result</t>
+  </si>
+  <si>
+    <t>Can do in O(1) space by iterating through parents while nodes not equal, set curr node to parent if its there, otherwise set it to the other original node</t>
+  </si>
+  <si>
+    <t>Score of a String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/score-of-a-string/submissions/1273778903/</t>
+  </si>
+  <si>
+    <t>Calculate sum by adding up absolute difference between adjacent pairs</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/basic-calculator-ii/submissions/1273940041/</t>
+  </si>
+  <si>
+    <t>Basic Calculator II</t>
+  </si>
+  <si>
+    <t>Use stack initially and handle all multiplication/division, then store in vector and do addition left to right</t>
+  </si>
+  <si>
+    <t>Better approach is stack of numbers and doing operations as you put it into stack</t>
+  </si>
+  <si>
+    <t>Nested List Weight Sum</t>
+  </si>
+  <si>
+    <t>DFS on list of lists, "Graph" only roughly fits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/nested-list-weight-sum/submissions/1274480972/</t>
+  </si>
+  <si>
+    <t>Loop over each n in list, if nested integer pass it recursively and keep looping, otherwise add to sum, keep track of depth</t>
+  </si>
+  <si>
+    <t>Reverse String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-string/submissions/1274641378/</t>
+  </si>
+  <si>
+    <t>L = 0, r = n-1, swap at each position</t>
+  </si>
+  <si>
+    <t>Random Pick With Weight</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/random-pick-with-weight/submissions/1274669550/</t>
+  </si>
+  <si>
+    <t>Store prefix sum, then do binary search over sum given random target in total sum to find right index</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-palindrome-ii/submissions/1274900066/</t>
+  </si>
+  <si>
+    <t>Valid Palindrome II</t>
+  </si>
+  <si>
+    <t>When chars differ, skip whatever maintains equality, if both are valid do the entire loop checking deleting both</t>
+  </si>
+  <si>
+    <t>Dot Product of Two Sparse Vectors</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/dot-product-of-two-sparse-vectors/submissions/1274915107/</t>
+  </si>
+  <si>
+    <t>Store non-zero indices, loop over them and multiply when inds btwn two vectors are equal w two pointers</t>
+  </si>
+  <si>
+    <t>Append Characters to String to Make Subsequence</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/append-characters-to-string-to-make-subsequence/submissions/1275828357/</t>
+  </si>
+  <si>
+    <t>Pointer on s,t, increment s and t when equal, when not increment s, at end take difference of t.size() and valid s increments</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-palindrome/submissions/1277156612/</t>
+  </si>
+  <si>
+    <t>Longest Palindrome</t>
+  </si>
+  <si>
+    <t>Don't have to use every character, misread question at first - BE PRECISE, EVEN ON EASIES</t>
+  </si>
+  <si>
+    <t>Count frequencies, for even add it to sum, for odds add (freq-1) and then fix offset at end if you took an odd</t>
+  </si>
+  <si>
+    <t>Length of Longest Valid Substring</t>
+  </si>
+  <si>
+    <t>Almost had right implementation, should've looked at constraints to fix TLE</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/length-of-the-longest-valid-substring/submissions/1277750778/</t>
+  </si>
+  <si>
+    <t>Make set of invalid words, do sliding window from end up till r or the max len of invalid word, keep pushing back letters and break if invalid while setting r to that index, always decrement l</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-common-characters/submissions/1278190009/</t>
+  </si>
+  <si>
+    <t>Find Common Characters</t>
+  </si>
+  <si>
+    <t>Keep map of (char+relative ind) to (count), push all values where frequency is equal to word list</t>
+  </si>
+  <si>
+    <t>Reorganize String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reorganize-string/submissions/1278930283/</t>
+  </si>
+  <si>
+    <t>Store pairs of freq,char, throw into desc PQ, keep placing max character by finding first valid position in string</t>
+  </si>
+  <si>
+    <t>Weird time complexity, basically n^2 * k loop in the end</t>
   </si>
 </sst>
 </file>
@@ -1791,10 +1947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:K136"/>
+  <dimension ref="A1:K151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+    <sheetView tabSelected="1" topLeftCell="C126" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H152" sqref="H152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5071,6 +5227,366 @@
       </c>
       <c r="G136" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>441</v>
+      </c>
+      <c r="B137" t="s">
+        <v>95</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D137" t="s">
+        <v>444</v>
+      </c>
+      <c r="E137" s="3">
+        <v>1</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G137" t="s">
+        <v>12</v>
+      </c>
+      <c r="H137" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>445</v>
+      </c>
+      <c r="B138" t="s">
+        <v>93</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="D138" t="s">
+        <v>447</v>
+      </c>
+      <c r="E138" s="3">
+        <v>1</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G138" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>448</v>
+      </c>
+      <c r="B139" t="s">
+        <v>93</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D139" t="s">
+        <v>450</v>
+      </c>
+      <c r="E139" s="3">
+        <v>1</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G139" t="s">
+        <v>161</v>
+      </c>
+      <c r="H139" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>452</v>
+      </c>
+      <c r="B140" t="s">
+        <v>95</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D140" t="s">
+        <v>454</v>
+      </c>
+      <c r="E140" s="3">
+        <v>1</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G140" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>456</v>
+      </c>
+      <c r="B141" t="s">
+        <v>93</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D141" t="s">
+        <v>457</v>
+      </c>
+      <c r="E141" s="3">
+        <v>1</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G141" t="s">
+        <v>340</v>
+      </c>
+      <c r="H141" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>459</v>
+      </c>
+      <c r="B142" t="s">
+        <v>93</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D142" t="s">
+        <v>462</v>
+      </c>
+      <c r="E142" s="3">
+        <v>1</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G142" t="s">
+        <v>16</v>
+      </c>
+      <c r="H142" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>463</v>
+      </c>
+      <c r="B143" t="s">
+        <v>95</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D143" t="s">
+        <v>465</v>
+      </c>
+      <c r="E143" s="3">
+        <v>1</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G143" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>466</v>
+      </c>
+      <c r="B144" t="s">
+        <v>93</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="D144" t="s">
+        <v>468</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G144" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>470</v>
+      </c>
+      <c r="B145" t="s">
+        <v>95</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D145" t="s">
+        <v>471</v>
+      </c>
+      <c r="E145" s="3">
+        <v>1</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G145" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>472</v>
+      </c>
+      <c r="B146" t="s">
+        <v>93</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D146" t="s">
+        <v>474</v>
+      </c>
+      <c r="E146" s="3">
+        <v>1</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G146" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>475</v>
+      </c>
+      <c r="B147" t="s">
+        <v>93</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="D147" t="s">
+        <v>477</v>
+      </c>
+      <c r="E147" s="3">
+        <v>1</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G147" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>479</v>
+      </c>
+      <c r="B148" t="s">
+        <v>95</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="D148" t="s">
+        <v>481</v>
+      </c>
+      <c r="E148" s="3">
+        <v>1</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G148" t="s">
+        <v>12</v>
+      </c>
+      <c r="H148" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>482</v>
+      </c>
+      <c r="B149" t="s">
+        <v>94</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="D149" t="s">
+        <v>485</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G149" t="s">
+        <v>34</v>
+      </c>
+      <c r="H149" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>487</v>
+      </c>
+      <c r="B150" t="s">
+        <v>95</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="D150" t="s">
+        <v>488</v>
+      </c>
+      <c r="E150" s="3">
+        <v>1</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G150" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>489</v>
+      </c>
+      <c r="B151" t="s">
+        <v>93</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D151" t="s">
+        <v>491</v>
+      </c>
+      <c r="E151" s="3">
+        <v>1</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G151" t="s">
+        <v>85</v>
+      </c>
+      <c r="H151" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -5128,6 +5644,21 @@
     <hyperlink ref="C134" r:id="rId40" xr:uid="{E400A34D-7519-274B-8AA6-BDC1F8381CE4}"/>
     <hyperlink ref="C135" r:id="rId41" xr:uid="{F8A0824E-0D06-5848-BBB1-1B4ABD266BCA}"/>
     <hyperlink ref="C136" r:id="rId42" xr:uid="{3806FC75-E461-1C40-AA11-26F63CE8E0A4}"/>
+    <hyperlink ref="C137" r:id="rId43" xr:uid="{69AF5EC6-2D24-5B45-A20E-C4340EA4EACB}"/>
+    <hyperlink ref="C138" r:id="rId44" xr:uid="{950DFCAF-2465-A14F-8A4F-264EF98B57EC}"/>
+    <hyperlink ref="C139" r:id="rId45" xr:uid="{F6CB1939-586E-4642-855A-2E89782EC064}"/>
+    <hyperlink ref="C140" r:id="rId46" xr:uid="{C7A4A740-9324-CE40-BDEA-B3862971D9E8}"/>
+    <hyperlink ref="C141" r:id="rId47" xr:uid="{C39FEED3-420A-2347-AB18-10A4D03122CD}"/>
+    <hyperlink ref="C142" r:id="rId48" xr:uid="{4C6278E4-D95C-9742-871F-E0BECE7FD76C}"/>
+    <hyperlink ref="C143" r:id="rId49" xr:uid="{6A2B70DF-7A78-C243-99A8-71FF973A0614}"/>
+    <hyperlink ref="C144" r:id="rId50" xr:uid="{80CE1920-6CC1-034A-A749-F496C9A66D54}"/>
+    <hyperlink ref="C145" r:id="rId51" xr:uid="{4026E9C8-06EF-1C4E-A69C-827F9E2A4F9D}"/>
+    <hyperlink ref="C146" r:id="rId52" xr:uid="{7C0B707A-6F1C-B74E-A785-11BAE37528A1}"/>
+    <hyperlink ref="C147" r:id="rId53" xr:uid="{EDC2107D-4131-DB4D-BF2A-617653BD25DA}"/>
+    <hyperlink ref="C148" r:id="rId54" xr:uid="{B583D815-7E07-6047-88A4-3FD2AD829E50}"/>
+    <hyperlink ref="C149" r:id="rId55" xr:uid="{8EAD7512-6EFE-CC4F-95ED-A134B0B21C58}"/>
+    <hyperlink ref="C150" r:id="rId56" xr:uid="{B347CCA4-D080-4149-9352-2D46DC313E82}"/>
+    <hyperlink ref="C151" r:id="rId57" xr:uid="{5C044441-041C-7641-B50F-6F484C4D1270}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 6/6
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEFE75C-79F2-1A43-B62C-638B18C62D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BD0BFD-1F09-0E45-95AB-60787D3C8DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="509">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1515,6 +1515,54 @@
   </si>
   <si>
     <t>Weird time complexity, basically n^2 * k loop in the end</t>
+  </si>
+  <si>
+    <t>Hand of Straights</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/hand-of-straights/submissions/1279261737/</t>
+  </si>
+  <si>
+    <t>Less optimal is greedy, just sort and build from group starting points</t>
+  </si>
+  <si>
+    <t>Create freq map, at each num in hand find starting point (where n-1 isn't in map) and see if you can make group</t>
+  </si>
+  <si>
+    <t>Sequential Digits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sequential-digits/submissions/1279274377/</t>
+  </si>
+  <si>
+    <t>Generate all possible sequential digits recursively, sort, and check which fits in range</t>
+  </si>
+  <si>
+    <t>More mem efficient to do sliding window approach on "123456789", avoids sorting</t>
+  </si>
+  <si>
+    <t>Buildings With An Ocean View</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/buildings-with-an-ocean-view/submissions/1279697013/</t>
+  </si>
+  <si>
+    <t>Go from end of arr, keep track of max and update as needed, if bldg &gt; max, add index</t>
+  </si>
+  <si>
+    <t>More interesting problem is stream of buildings, then can use stack</t>
+  </si>
+  <si>
+    <t>Subarray Sum Equals K</t>
+  </si>
+  <si>
+    <t>Initially did bf, n^2 brute force solution is trivial</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subarray-sum-equals-k/submissions/1279998163/</t>
+  </si>
+  <si>
+    <t>Map[sum-&gt;freq], loop through all nums and keep total sum, check if total_sum - k is in map and add freq to count, update map[sum] freq by 1</t>
   </si>
 </sst>
 </file>
@@ -1947,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:K151"/>
+  <dimension ref="A1:K155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C126" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H152" sqref="H152"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5587,6 +5635,110 @@
       </c>
       <c r="H151" t="s">
         <v>492</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>493</v>
+      </c>
+      <c r="B152" t="s">
+        <v>93</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="D152" t="s">
+        <v>496</v>
+      </c>
+      <c r="E152" s="3">
+        <v>1</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G152" t="s">
+        <v>12</v>
+      </c>
+      <c r="H152" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>497</v>
+      </c>
+      <c r="B153" t="s">
+        <v>93</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="D153" t="s">
+        <v>499</v>
+      </c>
+      <c r="E153" s="3">
+        <v>1</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G153" t="s">
+        <v>12</v>
+      </c>
+      <c r="H153" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>501</v>
+      </c>
+      <c r="B154" t="s">
+        <v>93</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="D154" t="s">
+        <v>503</v>
+      </c>
+      <c r="E154" s="3">
+        <v>1</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G154" t="s">
+        <v>12</v>
+      </c>
+      <c r="H154" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>505</v>
+      </c>
+      <c r="B155" t="s">
+        <v>93</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="D155" t="s">
+        <v>508</v>
+      </c>
+      <c r="E155" s="3">
+        <v>1</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G155" t="s">
+        <v>12</v>
+      </c>
+      <c r="H155" t="s">
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -5659,6 +5811,10 @@
     <hyperlink ref="C149" r:id="rId55" xr:uid="{8EAD7512-6EFE-CC4F-95ED-A134B0B21C58}"/>
     <hyperlink ref="C150" r:id="rId56" xr:uid="{B347CCA4-D080-4149-9352-2D46DC313E82}"/>
     <hyperlink ref="C151" r:id="rId57" xr:uid="{5C044441-041C-7641-B50F-6F484C4D1270}"/>
+    <hyperlink ref="C152" r:id="rId58" xr:uid="{82944DB5-D062-E64C-A50E-B801F143D948}"/>
+    <hyperlink ref="C153" r:id="rId59" xr:uid="{6E525A8C-9A5B-3E40-BF35-39C2E1025C97}"/>
+    <hyperlink ref="C154" r:id="rId60" xr:uid="{5DF08E26-6C23-8646-BA83-AE2D5CE70D1E}"/>
+    <hyperlink ref="C155" r:id="rId61" xr:uid="{C85B4ADD-4CC0-0448-AD80-E2BB7BD66E91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
LC Tracking - 6/28
</commit_message>
<xml_diff>
--- a/LeetcodeTracking.xlsx
+++ b/LeetcodeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarveshphoenix/Documents/Projects/Applications/Competitive Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B923C384-EBCF-594C-AC71-F34BC3162770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0CECC3-0A9C-2142-B5C8-CC14D7C4298F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{CB7727B8-EE7F-8D4B-915C-BB6765E35574}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="532">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1593,6 +1593,45 @@
   </si>
   <si>
     <t>Count item freq if in arr2, if not store in extra vector, push everything to vector then add stuff that wasn't found</t>
+  </si>
+  <si>
+    <t>Count Number of Nice Subarrays</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-number-of-nice-subarrays/submissions/1297073577/</t>
+  </si>
+  <si>
+    <t>Prefix sum approach, duplicate to Binary Continuous Array problem</t>
+  </si>
+  <si>
+    <t>Conver to 0s and 1s, count sum using hashmap and check if map[sum - target] in map</t>
+  </si>
+  <si>
+    <t>Find Center of Star Graph</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-center-of-star-graph/submissions/1301482812/</t>
+  </si>
+  <si>
+    <t>Count frequency of each number, whatever is equal to n must be center of graph</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/submissions/1301500416/</t>
+  </si>
+  <si>
+    <t>Keep hashset to show characters in current window, move r while valid, update max, then move left by 1</t>
+  </si>
+  <si>
+    <t>All Ancestors of a Node in a Directed Acyclic Graph</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/all-ancestors-of-a-node-in-a-directed-acyclic-graph/submissions/1303499521/</t>
+  </si>
+  <si>
+    <t>Make graph of reverse edges, for each number do a BFS and store all the ancestors</t>
   </si>
 </sst>
 </file>
@@ -2025,10 +2064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3920BFD-8DB2-E845-ADA2-11140478DC42}">
-  <dimension ref="A1:K158"/>
+  <dimension ref="A1:K162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A141" zoomScale="138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158"/>
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5841,6 +5880,101 @@
       </c>
       <c r="G158" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>519</v>
+      </c>
+      <c r="B159" t="s">
+        <v>93</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="D159" t="s">
+        <v>522</v>
+      </c>
+      <c r="E159" s="3">
+        <v>1</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G159" t="s">
+        <v>12</v>
+      </c>
+      <c r="H159" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>523</v>
+      </c>
+      <c r="B160" t="s">
+        <v>95</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="D160" t="s">
+        <v>525</v>
+      </c>
+      <c r="E160" s="3">
+        <v>1</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G160" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>526</v>
+      </c>
+      <c r="B161" t="s">
+        <v>93</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="D161" t="s">
+        <v>528</v>
+      </c>
+      <c r="E161" s="3">
+        <v>1</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G161" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>529</v>
+      </c>
+      <c r="B162" t="s">
+        <v>93</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="D162" t="s">
+        <v>531</v>
+      </c>
+      <c r="E162" s="3">
+        <v>1</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G162" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -5919,6 +6053,10 @@
     <hyperlink ref="C155" r:id="rId61" xr:uid="{C85B4ADD-4CC0-0448-AD80-E2BB7BD66E91}"/>
     <hyperlink ref="C157" r:id="rId62" xr:uid="{F16270A6-9F0F-CF49-8682-CFAE766E6A44}"/>
     <hyperlink ref="C158" r:id="rId63" xr:uid="{EDCAC1AF-405C-CE4D-BE0F-E2DA0DBE4B1A}"/>
+    <hyperlink ref="C159" r:id="rId64" xr:uid="{86D066FD-0084-E440-8FC6-1BADF6B5538D}"/>
+    <hyperlink ref="C160" r:id="rId65" xr:uid="{76A15CE3-7C6E-BC44-8650-DBDAB271D682}"/>
+    <hyperlink ref="C161" r:id="rId66" xr:uid="{4DD579EF-8239-AB4A-9089-23117F8C9F7B}"/>
+    <hyperlink ref="C162" r:id="rId67" xr:uid="{3C746F54-B0C8-5B4F-8C17-AD619FC47EA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>